<commit_message>
update : main manu
</commit_message>
<xml_diff>
--- a/doc/เธเธฒเธเธ—เนเธฒเน€เธฃเธทเธญ.xlsx
+++ b/doc/เธเธฒเธเธ—เนเธฒเน€เธฃเธทเธญ.xlsx
@@ -861,9 +861,6 @@
     <t>traffic-control</t>
   </si>
   <si>
-    <t>inspection</t>
-  </si>
-  <si>
     <t>warehouse</t>
   </si>
   <si>
@@ -880,6 +877,9 @@
   </si>
   <si>
     <t>transfer</t>
+  </si>
+  <si>
+    <t>counting</t>
   </si>
 </sst>
 </file>
@@ -2985,7 +2985,7 @@
   <dimension ref="A2:H84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.5"/>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="D18" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E18" s="42" t="s">
         <v>263</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.5">
       <c r="D65" s="9" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="E65" s="31" t="s">
         <v>220</v>
@@ -3733,7 +3733,7 @@
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.5">
       <c r="D69" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E69" s="26" t="s">
         <v>227</v>
@@ -3774,7 +3774,7 @@
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.5">
       <c r="D73" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E73" s="29" t="s">
         <v>233</v>
@@ -3815,7 +3815,7 @@
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.5">
       <c r="D77" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E77" s="31" t="s">
         <v>241</v>
@@ -3848,7 +3848,7 @@
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.5">
       <c r="D80" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E80" s="26" t="s">
         <v>246</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.5">
       <c r="D84" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E84" s="31" t="s">
         <v>254</v>

</xml_diff>

<commit_message>
update : js manu
</commit_message>
<xml_diff>
--- a/doc/เธเธฒเธเธ—เนเธฒเน€เธฃเธทเธญ.xlsx
+++ b/doc/เธเธฒเธเธ—เนเธฒเน€เธฃเธทเธญ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="289">
   <si>
     <t>รายการ</t>
   </si>
@@ -880,6 +880,9 @@
   </si>
   <si>
     <t>counting</t>
+  </si>
+  <si>
+    <t>ผู้ใช้งานในระบบ</t>
   </si>
 </sst>
 </file>
@@ -2984,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.5"/>
@@ -3134,7 +3137,7 @@
         <v>98</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>95</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>